<commit_message>
1) Added wait method 				2)Browser version update 				3)Navigation to content Analysis				4)Added class to run the application				5) POM Library						6) POM Library					7) Added test				8)Created new filename				9)Added vendors
</commit_message>
<xml_diff>
--- a/data/VendorList.xlsx
+++ b/data/VendorList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F5EAB2-5ED1-4D1D-9312-137F837B5E9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB3822B-B6B5-4232-93E3-9745805D123C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Facebook</t>
   </si>
@@ -80,25 +80,14 @@
   </si>
   <si>
     <t>Zomato</t>
-  </si>
-  <si>
-    <t>VendorList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,10 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,9 +419,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -442,106 +432,101 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
+      <c r="A8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="A9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="A11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
+      <c r="A13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
+      <c r="A14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
+      <c r="A15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
+      <c r="A17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1)Updated Chrome Browser 				2)Added wait					3)Navigate to Google Ranking					 4)Added Test to run Google Ranking 					5)Changes made to check vendors 					6)Changes made if data is not available in table 					7)Added a test case to compare UI and Excel 					8)Changes made if data is not available in table 			9)Added a test case to compare UI and Excel 					10)Changes made if data is not available in table 					11)Added a test case to compare UI and Excel 					12)Changes made if data is not available in table 					13)Added a test case to compare UI and Excel	 				14)Added code to rename excel file 					15)Added Vendor List in Excel
</commit_message>
<xml_diff>
--- a/data/VendorList.xlsx
+++ b/data/VendorList.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB3822B-B6B5-4232-93E3-9745805D123C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BCD50FA1-773E-4EEC-A187-D52A96133772}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="VendorList" sheetId="1" r:id="rId1"/>
+    <sheet name="VendorList" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Facebook</t>
   </si>
@@ -56,27 +56,6 @@
   </si>
   <si>
     <t>OpenTable</t>
-  </si>
-  <si>
-    <t>YP.ca</t>
-  </si>
-  <si>
-    <t>Touch Local</t>
-  </si>
-  <si>
-    <t>YahooUK</t>
-  </si>
-  <si>
-    <t>Mappy</t>
-  </si>
-  <si>
-    <t>PagesJaunes</t>
-  </si>
-  <si>
-    <t>Scoot</t>
-  </si>
-  <si>
-    <t>Yell</t>
   </si>
   <si>
     <t>Zomato</t>
@@ -86,6 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,17 +114,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -161,10 +141,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -199,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -234,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -328,21 +308,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -359,7 +339,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -411,23 +391,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -495,43 +475,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1)Removed unwanted imports					2)Removed unwanted imports						3)Removed unwanted imports					4)Removed unwanted imports					5)Removed unwanted imports					6)Removed unwanted imports					7)Removed unwanted imports					8)Changed user to login					9)Removed unwanted imports					10)Removed unwanted imports					11)Added dependency to take full page screenshot					12)Created methods to get KPI values					13)Added methods to export of pdf 					14)Added testcases for export as pdf					15)Added name for pdf					16)Updated vendor list
</commit_message>
<xml_diff>
--- a/data/VendorList.xlsx
+++ b/data/VendorList.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{BCD50FA1-773E-4EEC-A187-D52A96133772}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF75DC17-0084-4C79-8743-8E8429F62BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VendorList" r:id="rId1" sheetId="1"/>
+    <sheet name="VendorList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Facebook</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Bing</t>
   </si>
   <si>
-    <t>Citysearch</t>
-  </si>
-  <si>
-    <t>MerchantCircle</t>
-  </si>
-  <si>
     <t>Superpages</t>
   </si>
   <si>
@@ -55,17 +49,37 @@
     <t>TripAdvisor</t>
   </si>
   <si>
-    <t>OpenTable</t>
-  </si>
-  <si>
-    <t>Zomato</t>
+    <t>YP.ca</t>
+  </si>
+  <si>
+    <t>Touch Local</t>
+  </si>
+  <si>
+    <t>Scoot</t>
+  </si>
+  <si>
+    <t>Yell</t>
+  </si>
+  <si>
+    <t>All Sites</t>
+  </si>
+  <si>
+    <t>Search Engine Sites</t>
+  </si>
+  <si>
+    <t>Directory Sites</t>
+  </si>
+  <si>
+    <t>Social Sites</t>
+  </si>
+  <si>
+    <t>YahooUK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,21 +89,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -112,19 +134,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -141,10 +177,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -179,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -214,7 +250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -308,21 +344,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -339,7 +375,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -391,92 +427,208 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1)Updated Vendor List					2)Updated history pdf export method
</commit_message>
<xml_diff>
--- a/data/VendorList.xlsx
+++ b/data/VendorList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF75DC17-0084-4C79-8743-8E8429F62BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44CF75-97B1-40B4-9B28-D6E4D98F5B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Facebook</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>YahooUK</t>
+  </si>
+  <si>
+    <t>Yahoo UK</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,27 +137,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +430,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +456,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -478,7 +470,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -490,7 +482,7 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -502,17 +494,19 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
@@ -522,7 +516,7 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4"/>
@@ -532,7 +526,7 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4"/>
@@ -542,7 +536,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4"/>
@@ -552,7 +546,7 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4"/>
@@ -562,7 +556,7 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="4"/>
@@ -572,7 +566,7 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4"/>
@@ -580,7 +574,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
@@ -588,7 +582,7 @@
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4"/>
@@ -596,7 +590,7 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="4"/>

</xml_diff>